<commit_message>
alterações conexão front e modelagem do banco
</commit_message>
<xml_diff>
--- a/DOCUMENTAÇÃO/Backlog_KnowFootball.xlsx
+++ b/DOCUMENTAÇÃO/Backlog_KnowFootball.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/04395b400f7f60cb/Desktop/Projeto knowfootball/Projeto_Matheus_Valle_know-football/DOCUMENTAÇÃO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="8_{4B7EDD68-DCB0-4DD0-A779-2F4742B46CC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5E432283-DCC9-43B4-AE44-4D6790D25968}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="8_{4B7EDD68-DCB0-4DD0-A779-2F4742B46CC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0025E8F2-BB56-4977-84B9-DE4F350CA595}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{5CE54B8C-27E7-43A3-A284-970DD8A8DBF5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5CE54B8C-27E7-43A3-A284-970DD8A8DBF5}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -549,11 +549,42 @@
           <c:cat>
             <c:strRef>
               <c:f>Planilha1!$P$5:$P$8</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>TOTAL</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>SP3A</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>SP3B</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>SP3C</c:v>
+                </c:pt>
+              </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Planilha1!$Q$5:$Q$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>258</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>70</c:v>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
@@ -571,7 +602,6 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
         <c:axId val="1783834815"/>
         <c:axId val="1783838175"/>
@@ -832,7 +862,7 @@
               <c:f>Planilha1!$R$21:$R$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>258</c:v>
                 </c:pt>
@@ -841,6 +871,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>70</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -883,7 +916,7 @@
               <c:f>Planilha1!$S$21:$S$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>62</c:v>
                 </c:pt>
@@ -2611,10 +2644,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{038C9E5A-C559-4D5A-AF1D-688BEFA4C9AC}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:T30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
@@ -2668,7 +2700,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>44</v>
       </c>
@@ -2699,7 +2731,7 @@
       <c r="Q3" s="12"/>
       <c r="R3" s="12"/>
     </row>
-    <row r="4" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="13"/>
       <c r="B4" s="2" t="s">
         <v>10</v>
@@ -2730,7 +2762,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="13"/>
       <c r="B5" s="2" t="s">
         <v>11</v>
@@ -2763,7 +2795,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="6" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="13"/>
       <c r="B6" s="2" t="s">
         <v>12</v>
@@ -2796,7 +2828,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="7" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="13"/>
       <c r="B7" s="2" t="s">
         <v>13</v>
@@ -2829,7 +2861,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="8" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="13"/>
       <c r="B8" s="2" t="s">
         <v>14</v>
@@ -2862,7 +2894,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="13"/>
       <c r="B9" s="2" t="s">
         <v>15</v>
@@ -2886,7 +2918,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="13"/>
       <c r="B10" s="2" t="s">
         <v>43</v>
@@ -2910,7 +2942,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="13"/>
       <c r="B11" s="2" t="s">
         <v>81</v>
@@ -2934,7 +2966,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="14" t="s">
         <v>49</v>
       </c>
@@ -2960,7 +2992,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="14"/>
       <c r="B13" s="4" t="s">
         <v>33</v>
@@ -2984,7 +3016,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="14"/>
       <c r="B14" s="4" t="s">
         <v>34</v>
@@ -3008,7 +3040,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="15" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
       <c r="B15" s="4" t="s">
         <v>35</v>
@@ -3032,7 +3064,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="14"/>
       <c r="B16" s="4" t="s">
         <v>36</v>
@@ -3056,7 +3088,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" s="14"/>
       <c r="B17" s="4" t="s">
         <v>37</v>
@@ -3080,7 +3112,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="18" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" s="14"/>
       <c r="B18" s="4" t="s">
         <v>38</v>
@@ -3104,7 +3136,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19" s="14"/>
       <c r="B19" s="4" t="s">
         <v>39</v>
@@ -3135,7 +3167,7 @@
       <c r="S19" s="12"/>
       <c r="T19" s="12"/>
     </row>
-    <row r="20" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20" s="14"/>
       <c r="B20" s="4" t="s">
         <v>40</v>
@@ -3285,7 +3317,7 @@
       <c r="S23" s="8"/>
       <c r="T23" s="9"/>
     </row>
-    <row r="24" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A24" s="14"/>
       <c r="B24" s="4" t="s">
         <v>47</v>
@@ -3400,13 +3432,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="H2:H27" xr:uid="{038C9E5A-C559-4D5A-AF1D-688BEFA4C9AC}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="3C"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="H2:H27" xr:uid="{038C9E5A-C559-4D5A-AF1D-688BEFA4C9AC}"/>
   <mergeCells count="6">
     <mergeCell ref="A26:A27"/>
     <mergeCell ref="A1:H1"/>

</xml_diff>